<commit_message>
3D rendering (Not working; WIP)
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="20" windowWidth="27640" windowHeight="17200"/>
+    <workbookView xWindow="4720" yWindow="1460" windowWidth="27640" windowHeight="17200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -366,6 +366,9 @@
   </si>
   <si>
     <t>Student Git Address: https://github.com/Mush-kinn/GraphicsII_FS.git</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -946,7 +949,7 @@
   <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1061,7 +1064,9 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G30" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
@@ -3023,7 +3028,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>